<commit_message>
Last changes for Cassia
</commit_message>
<xml_diff>
--- a/data/plains.xlsx
+++ b/data/plains.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="143">
   <si>
     <t xml:space="preserve">RFID</t>
   </si>
@@ -31,10 +31,16 @@
     <t xml:space="preserve">QUANTIDADE</t>
   </si>
   <si>
+    <t xml:space="preserve">D61E3C1E</t>
+  </si>
+  <si>
     <t xml:space="preserve">BOB ALUM 0,10X688,8MM</t>
   </si>
   <si>
-    <t xml:space="preserve">DESENGRAXANTE PARCO CLEANER</t>
+    <t xml:space="preserve">BC964FD3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASSIANA UNICORNIO</t>
   </si>
   <si>
     <t xml:space="preserve">A04807101</t>
@@ -524,7 +530,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -533,16 +539,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -565,7 +567,7 @@
   <dimension ref="A1:C95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -588,66 +590,66 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>62494132</v>
+      <c r="A2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
-        <v>63091111</v>
+      <c r="A3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>100</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>7</v>
+      <c r="A5" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
+      <c r="A6" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
+      <c r="A7" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>55</v>
@@ -658,7 +660,7 @@
         <v>69390048</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>55</v>
@@ -669,7 +671,7 @@
         <v>62291712</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>8</v>
@@ -677,10 +679,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>8</v>
@@ -691,7 +693,7 @@
         <v>68190243</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>98</v>
@@ -702,7 +704,7 @@
         <v>63091117</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>5</v>
@@ -713,7 +715,7 @@
         <v>63199515</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>77</v>
@@ -721,10 +723,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>8</v>
@@ -735,7 +737,7 @@
         <v>69000040</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>23</v>
@@ -743,10 +745,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>67</v>
@@ -757,7 +759,7 @@
         <v>62291535</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>43</v>
@@ -765,10 +767,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>4</v>
@@ -776,10 +778,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>6</v>
@@ -787,10 +789,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>9</v>
@@ -798,10 +800,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>545</v>
@@ -809,10 +811,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>87</v>
@@ -823,7 +825,7 @@
         <v>68000609</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>564</v>
@@ -831,10 +833,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>2</v>
@@ -842,10 +844,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>3</v>
@@ -853,10 +855,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>45</v>
@@ -867,7 +869,7 @@
         <v>63490206</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>4</v>
@@ -878,7 +880,7 @@
         <v>69000766</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>8</v>
@@ -886,10 +888,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>7</v>
@@ -900,7 +902,7 @@
         <v>63000228</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>5</v>
@@ -911,7 +913,7 @@
         <v>67402457</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>86</v>
@@ -919,10 +921,10 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>45</v>
@@ -933,7 +935,7 @@
         <v>62000683</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>645</v>
@@ -941,10 +943,10 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>2</v>
@@ -955,7 +957,7 @@
         <v>62000694</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>45</v>
@@ -966,7 +968,7 @@
         <v>62000685</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>2</v>
@@ -974,10 +976,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>21</v>
@@ -988,7 +990,7 @@
         <v>98102011</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>4</v>
@@ -999,7 +1001,7 @@
         <v>67402439</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>4</v>
@@ -1010,7 +1012,7 @@
         <v>98100201</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>5</v>
@@ -1021,7 +1023,7 @@
         <v>62000696</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>4</v>
@@ -1029,10 +1031,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>8</v>
@@ -1043,7 +1045,7 @@
         <v>62000681</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C43" s="2" t="n">
         <v>7</v>
@@ -1051,10 +1053,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C44" s="2" t="n">
         <v>5</v>
@@ -1062,10 +1064,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C45" s="2" t="n">
         <v>86</v>
@@ -1076,7 +1078,7 @@
         <v>9818002</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C46" s="2" t="n">
         <v>45</v>
@@ -1084,10 +1086,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C47" s="2" t="n">
         <v>645</v>
@@ -1095,10 +1097,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C48" s="2" t="n">
         <v>2</v>
@@ -1106,32 +1108,32 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C49" s="2" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
-        <v>63</v>
+      <c r="A50" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C50" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
-        <v>65</v>
+      <c r="A51" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C51" s="2" t="n">
         <v>21</v>
@@ -1139,10 +1141,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C52" s="2" t="n">
         <v>4</v>
@@ -1153,7 +1155,7 @@
         <v>62093723</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C53" s="2" t="n">
         <v>4</v>
@@ -1164,7 +1166,7 @@
         <v>62093724</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C54" s="2" t="n">
         <v>5</v>
@@ -1175,7 +1177,7 @@
         <v>63000333</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C55" s="2" t="n">
         <v>3</v>
@@ -1183,10 +1185,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C56" s="2" t="n">
         <v>45</v>
@@ -1194,10 +1196,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C57" s="2" t="n">
         <v>4</v>
@@ -1205,10 +1207,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C58" s="2" t="n">
         <v>8</v>
@@ -1216,10 +1218,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C59" s="2" t="n">
         <v>7</v>
@@ -1230,7 +1232,7 @@
         <v>69001235</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C60" s="2" t="n">
         <v>5</v>
@@ -1238,10 +1240,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C61" s="2" t="n">
         <v>86</v>
@@ -1252,7 +1254,7 @@
         <v>72002015</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C62" s="2" t="n">
         <v>45</v>
@@ -1263,7 +1265,7 @@
         <v>72002017</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C63" s="2" t="n">
         <v>645</v>
@@ -1274,7 +1276,7 @@
         <v>72002018</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C64" s="2" t="n">
         <v>2</v>
@@ -1285,7 +1287,7 @@
         <v>72002019</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C65" s="2" t="n">
         <v>45</v>
@@ -1293,10 +1295,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C66" s="2" t="n">
         <v>2</v>
@@ -1304,10 +1306,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C67" s="2" t="n">
         <v>21</v>
@@ -1315,10 +1317,10 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C68" s="2" t="n">
         <v>4</v>
@@ -1326,10 +1328,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C69" s="2" t="n">
         <v>4</v>
@@ -1337,21 +1339,21 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C70" s="2" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4" t="s">
-        <v>94</v>
+      <c r="A71" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C71" s="2" t="n">
         <v>4</v>
@@ -1359,10 +1361,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C72" s="2" t="n">
         <v>8</v>
@@ -1370,10 +1372,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C73" s="2" t="n">
         <v>7</v>
@@ -1381,10 +1383,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C74" s="2" t="n">
         <v>5</v>
@@ -1392,10 +1394,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C75" s="2" t="n">
         <v>4</v>
@@ -1403,10 +1405,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C76" s="2" t="n">
         <v>6</v>
@@ -1414,10 +1416,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C77" s="2" t="n">
         <v>9</v>
@@ -1425,10 +1427,10 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C78" s="2" t="n">
         <v>545</v>
@@ -1436,10 +1438,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C79" s="2" t="n">
         <v>87</v>
@@ -1447,10 +1449,10 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C80" s="2" t="n">
         <v>564</v>
@@ -1458,10 +1460,10 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C81" s="2" t="n">
         <v>2</v>
@@ -1469,10 +1471,10 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C82" s="2" t="n">
         <v>3</v>
@@ -1480,10 +1482,10 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C83" s="2" t="n">
         <v>45</v>
@@ -1491,10 +1493,10 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C84" s="2" t="n">
         <v>4</v>
@@ -1502,10 +1504,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C85" s="2" t="n">
         <v>8</v>
@@ -1513,10 +1515,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C86" s="2" t="n">
         <v>7</v>
@@ -1524,10 +1526,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C87" s="2" t="n">
         <v>5</v>
@@ -1535,10 +1537,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C88" s="2" t="n">
         <v>86</v>
@@ -1546,10 +1548,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C89" s="2" t="n">
         <v>45</v>
@@ -1557,10 +1559,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C90" s="2" t="n">
         <v>645</v>
@@ -1568,10 +1570,10 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C91" s="2" t="n">
         <v>2</v>
@@ -1579,10 +1581,10 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C92" s="2" t="n">
         <v>45</v>
@@ -1590,10 +1592,10 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C93" s="2" t="n">
         <v>2</v>
@@ -1601,10 +1603,10 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C94" s="2" t="n">
         <v>21</v>
@@ -1615,7 +1617,7 @@
         <v>67402546</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C95" s="2" t="n">
         <v>4</v>

</xml_diff>